<commit_message>
updating inputs and some fixes on potential inputs
</commit_message>
<xml_diff>
--- a/optimized_study_plan.xlsx
+++ b/optimized_study_plan.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,34 +457,34 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Article Review</t>
+          <t>Mat. Modelling - Midterm</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Project1</t>
+          <t xml:space="preserve">Mat. Modelling - Assignment 1 </t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -493,52 +493,52 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Midterm</t>
+          <t xml:space="preserve">Mat. Modelling - Assignment 1 </t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Project1</t>
+          <t>Logistics - 1-4th week review</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Project1</t>
+          <t>S.C. Analytical Methods - Midterm</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -547,169 +547,169 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>S.C. Analytical Methods - Midterm</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>3</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Midterm</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Midterm</t>
+          <t>Mat. Modelling - Midterm</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Project2</t>
+          <t xml:space="preserve">S.C. Analytical Methods - Project Proposal </t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t xml:space="preserve">S.C. Analytical Methods - Project Proposal </t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Midterm</t>
+          <t>S.C. Analytical Methods - Project Proposal 2</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Project2</t>
+          <t>Logistics - Midterm</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Logistics - Midterm</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mat. Modelling - Project Report 1 </t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>5</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Article Review</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Project2</t>
+          <t>Logistics - 4-8th week review</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -718,16 +718,16 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Mat. Modelling - Assignment 2</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -736,16 +736,16 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Mat. Modelling - Assignment 2</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>S.C. Analytical Methods - Final</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -763,7 +763,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -772,25 +772,25 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>Logistics - 4-8th week review</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>S.C. Analytical Methods - Project Proposal 2</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -803,34 +803,448 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Final</t>
+          <t>S.C. Analytical Methods - Project Proposal 2</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Mat. Modelling - Midterm</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>9</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mat. Modelling - Project Report 2 &amp; Presentation </t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>9</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>S.C. Analytical Methods - Final</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>9</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>Sunday</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Final</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>8</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Logistics - 8-10th week review</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>10</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>S.C. Analytical Methods - Project Proposal 2</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>11</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mat. Modelling - Project Report 2 &amp; Presentation </t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>11</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Mat. Modelling - Final</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>12</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Mat. Modelling - Assignment 3</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>12</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mat. Modelling - Project Report 2 &amp; Presentation </t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>12</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>S.C. Analytical Methods - Project Proposal 2</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>12</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Logistics - 10-12th week review</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>12</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Mat. Modelling - Assignment 3</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>12</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mat. Modelling - Project Report 2 &amp; Presentation </t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>14</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Mat. Modelling - Final</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>14</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Mat. Modelling - Final</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>14</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mat. Modelling - Project Report 2 &amp; Presentation </t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>14</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Logistics - 12-14th week review</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>14</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>S.C. Analytical Methods - Final</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>14</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>S.C. Analytical Methods - Final</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>14</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>S.C. Analytical Methods - Paper Review Presentation</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>15</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Logistics - Final</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>15</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Logistics - Final</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>15</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>S.C. Analytical Methods - Final</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>16</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Logistics - Final</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>